<commit_message>
FAAS-797 - Error Specs
</commit_message>
<xml_diff>
--- a/src/test/resources/FHEO-Testdata1.xlsx
+++ b/src/test/resources/FHEO-Testdata1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B662D7BD-2430-4D1B-8473-24063D2B0C4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5486BBEF-876B-4006-81E0-F73BFE91FC11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,25 +195,25 @@
     <t>JohnMS@gmail.com</t>
   </si>
   <si>
-    <t>Smith1</t>
-  </si>
-  <si>
     <t>Washington, D.C.</t>
   </si>
   <si>
-    <t>John1</t>
-  </si>
-  <si>
     <t>District of Columbia</t>
   </si>
   <si>
     <t>Akil1@gmail.com</t>
   </si>
   <si>
-    <t>Krish - Auto1</t>
-  </si>
-  <si>
-    <t>Updik1</t>
+    <t>Krish - Auto6</t>
+  </si>
+  <si>
+    <t>Smith6</t>
+  </si>
+  <si>
+    <t>John6</t>
+  </si>
+  <si>
+    <t>Updik6</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1159,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD51"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1318,8 +1318,8 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="19" t="s">
-        <v>6</v>
+      <c r="A2" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
@@ -1333,17 +1333,17 @@
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>7</v>
+      <c r="F2" s="19" t="s">
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>10</v>
@@ -1352,10 +1352,10 @@
         <v>8009098909</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>23</v>
@@ -1379,7 +1379,7 @@
         <v>27</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="W2" s="13" t="s">
         <v>60</v>
@@ -1400,7 +1400,7 @@
         <v>45</v>
       </c>
       <c r="AC2" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD2" s="13" t="s">
         <v>22</v>
@@ -1430,9 +1430,9 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{37BC02B3-4843-49B6-B6BB-BF0B530FC773}"/>
-    <hyperlink ref="AK2" r:id="rId2" xr:uid="{D863FA20-D542-4FBC-A59A-E8A7413D0C6A}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{B59FDA4B-C7C8-4441-8F17-326054B92699}"/>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{2B91F473-37EF-43D6-919A-EAE0BDB0C9FD}"/>
+    <hyperlink ref="AK2" r:id="rId2" xr:uid="{1B556879-DC18-4AA5-9AA1-51D05DC8F4C0}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{AC75280C-1B75-448E-9BFC-CF5283A11E18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>